<commit_message>
More metadata and Attribute edits
</commit_message>
<xml_diff>
--- a/Spatial_data/UVic/Harrop-Archibald 2008/Rootballs/Rootball Metadata.xlsx
+++ b/Spatial_data/UVic/Harrop-Archibald 2008/Rootballs/Rootball Metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Documents\GitHub\Github Shackelford-lab\Shackelford-lab\Spatial_data\UVic\Harrop-Archibald 2008\rootball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Documents\GitHub\Github Shackelford-lab\Shackelford-lab\Spatial_data\UVic\Harrop-Archibald 2008\Rootballs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FBEA2B-C1C8-4527-9F77-1728D43DEC06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E65E48-D55B-4E9E-99FA-4C242BF57C3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="2385" windowWidth="17400" windowHeight="10785" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
+    <workbookView xWindow="10110" yWindow="300" windowWidth="14970" windowHeight="14595" xr2:uid="{6934027C-8984-4F11-9C55-B9A1F75C2751}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Data table metadata</t>
   </si>
@@ -84,22 +84,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Date that the point was gathered. </t>
-  </si>
-  <si>
-    <t>yyyy-mm-dd</t>
-  </si>
-  <si>
-    <t>Year-month-day
-E.g. 2008-11-29</t>
-  </si>
-  <si>
-    <t>18-06-2020</t>
-  </si>
-  <si>
-    <t>Varied</t>
-  </si>
-  <si>
     <t>Garry Oak Points</t>
   </si>
   <si>
@@ -110,13 +94,106 @@
   </si>
   <si>
     <t>Numeric value for each point.</t>
+  </si>
+  <si>
+    <t>23-06-2020</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Year the data was recorded.</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Values:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+yyyy. E.g. 2008. 
+NULL = neither the original meta-data nor accompanying report gave the year of creation. </t>
+    </r>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Month the data was recorded.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Values:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1-12. E.g. 2=February.
+NULL = neither the original meta-data nor accompanying report gave the month of creation. </t>
+    </r>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Day the data was recorded.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Values:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1-31. E.g. 15=the 15th day of a month. 
+NULL = neither the original meta-data nor accompanying report gave the day of creation.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +227,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -210,16 +294,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -537,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC2632A-81E2-4372-B21A-08C497B1BE35}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,27 +635,27 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -582,7 +666,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -593,7 +677,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -604,78 +688,78 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" s="9" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
+      <c r="B9" s="11">
+        <v>2007</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="4">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3"/>
@@ -683,8 +767,8 @@
       <c r="E12" s="3"/>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1"/>
@@ -715,32 +799,69 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="9" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" s="9" customFormat="1" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" s="9" customFormat="1" ht="72.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>